<commit_message>
working on importing the data from exel file
</commit_message>
<xml_diff>
--- a/student.xlsx
+++ b/student.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I103"/>
+  <dimension ref="A1:I205"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -490,7 +490,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>7083</v>
+        <v>101</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -500,9 +500,7 @@
       <c r="F2" t="n">
         <v>100</v>
       </c>
-      <c r="G2" t="n">
-        <v>100</v>
-      </c>
+      <c r="G2" t="inlineStr"/>
       <c r="H2" t="n">
         <v>100</v>
       </c>
@@ -551,7 +549,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Raj khadka</t>
+          <t>raj khadka</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -560,7 +558,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>7224</v>
+        <v>102</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -568,16 +566,14 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>45</v>
-      </c>
-      <c r="G4" t="n">
-        <v>73</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="G4" t="inlineStr"/>
       <c r="H4" t="n">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="I4" t="n">
-        <v>18</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5">
@@ -4141,6 +4137,3675 @@
         <v>61</v>
       </c>
       <c r="I103" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="n">
+        <v>102</v>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>sarthak kafle</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>ithari-2</t>
+        </is>
+      </c>
+      <c r="D104" t="n">
+        <v>101</v>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="F104" t="n">
+        <v>100</v>
+      </c>
+      <c r="G104" t="n">
+        <v>0</v>
+      </c>
+      <c r="H104" t="n">
+        <v>100</v>
+      </c>
+      <c r="I104" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="n">
+        <v>103</v>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>John Doe</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>123 Main St</t>
+        </is>
+      </c>
+      <c r="D105" t="n">
+        <v>1</v>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="F105" t="n">
+        <v>85</v>
+      </c>
+      <c r="G105" t="n">
+        <v>90</v>
+      </c>
+      <c r="H105" t="n">
+        <v>95</v>
+      </c>
+      <c r="I105" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="n">
+        <v>104</v>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>raj khadka</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>budhanilkantha</t>
+        </is>
+      </c>
+      <c r="D106" t="n">
+        <v>102</v>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="F106" t="n">
+        <v>40</v>
+      </c>
+      <c r="G106" t="n">
+        <v>0</v>
+      </c>
+      <c r="H106" t="n">
+        <v>40</v>
+      </c>
+      <c r="I106" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="n">
+        <v>105</v>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>Kristen Alexander</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>4747 Simpson Burgs Apt. 698
+Annachester, AZ 09085</t>
+        </is>
+      </c>
+      <c r="D107" t="n">
+        <v>71</v>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="F107" t="n">
+        <v>82</v>
+      </c>
+      <c r="G107" t="n">
+        <v>76</v>
+      </c>
+      <c r="H107" t="n">
+        <v>90</v>
+      </c>
+      <c r="I107" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="n">
+        <v>106</v>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Lindsey Johnson</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>52545 Eaton Course
+East Kimberly, MN 71634</t>
+        </is>
+      </c>
+      <c r="D108" t="n">
+        <v>34</v>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="F108" t="n">
+        <v>84</v>
+      </c>
+      <c r="G108" t="n">
+        <v>64</v>
+      </c>
+      <c r="H108" t="n">
+        <v>57</v>
+      </c>
+      <c r="I108" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="n">
+        <v>107</v>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>Alicia Wu</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>12118 York Green Suite 363
+West Stacyfurt, TN 63621</t>
+        </is>
+      </c>
+      <c r="D109" t="n">
+        <v>70</v>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="F109" t="n">
+        <v>75</v>
+      </c>
+      <c r="G109" t="n">
+        <v>41</v>
+      </c>
+      <c r="H109" t="n">
+        <v>83</v>
+      </c>
+      <c r="I109" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="1" t="n">
+        <v>108</v>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>Pamela Bender</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>USS Gonzales
+FPO AP 11394</t>
+        </is>
+      </c>
+      <c r="D110" t="n">
+        <v>24</v>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="F110" t="n">
+        <v>91</v>
+      </c>
+      <c r="G110" t="n">
+        <v>47</v>
+      </c>
+      <c r="H110" t="n">
+        <v>86</v>
+      </c>
+      <c r="I110" t="n">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="1" t="n">
+        <v>109</v>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>Christopher Dunlap</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>Unit 9999 Box 7953
+DPO AE 19418</t>
+        </is>
+      </c>
+      <c r="D111" t="n">
+        <v>73</v>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="F111" t="n">
+        <v>69</v>
+      </c>
+      <c r="G111" t="n">
+        <v>100</v>
+      </c>
+      <c r="H111" t="n">
+        <v>44</v>
+      </c>
+      <c r="I111" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>Kevin Bowen</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>231 Richard Flats Suite 198
+West Stephanieport, MN 40085</t>
+        </is>
+      </c>
+      <c r="D112" t="n">
+        <v>97</v>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="F112" t="n">
+        <v>60</v>
+      </c>
+      <c r="G112" t="n">
+        <v>47</v>
+      </c>
+      <c r="H112" t="n">
+        <v>54</v>
+      </c>
+      <c r="I112" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="1" t="n">
+        <v>111</v>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>Thomas Steele</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>214 Williams Lodge
+West Brent, LA 07058</t>
+        </is>
+      </c>
+      <c r="D113" t="n">
+        <v>28</v>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="F113" t="n">
+        <v>63</v>
+      </c>
+      <c r="G113" t="n">
+        <v>76</v>
+      </c>
+      <c r="H113" t="n">
+        <v>85</v>
+      </c>
+      <c r="I113" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="1" t="n">
+        <v>112</v>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>Adrian Williamson</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>6224 Jones Plaza Apt. 853
+Erinmouth, CA 83009</t>
+        </is>
+      </c>
+      <c r="D114" t="n">
+        <v>94</v>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="F114" t="n">
+        <v>53</v>
+      </c>
+      <c r="G114" t="n">
+        <v>76</v>
+      </c>
+      <c r="H114" t="n">
+        <v>56</v>
+      </c>
+      <c r="I114" t="n">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="1" t="n">
+        <v>113</v>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>George Wu</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>73487 Casey Square
+New Sandrachester, MD 95762</t>
+        </is>
+      </c>
+      <c r="D115" t="n">
+        <v>58</v>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="F115" t="n">
+        <v>56</v>
+      </c>
+      <c r="G115" t="n">
+        <v>92</v>
+      </c>
+      <c r="H115" t="n">
+        <v>100</v>
+      </c>
+      <c r="I115" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="1" t="n">
+        <v>114</v>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>Bonnie Perez</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>901 Kimberly Stream Suite 176
+Amandahaven, TN 41841</t>
+        </is>
+      </c>
+      <c r="D116" t="n">
+        <v>93</v>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="F116" t="n">
+        <v>54</v>
+      </c>
+      <c r="G116" t="n">
+        <v>44</v>
+      </c>
+      <c r="H116" t="n">
+        <v>75</v>
+      </c>
+      <c r="I116" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="1" t="n">
+        <v>115</v>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>Jodi Taylor MD</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>67246 Mary Terrace
+Winterschester, CO 28430</t>
+        </is>
+      </c>
+      <c r="D117" t="n">
+        <v>51</v>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="F117" t="n">
+        <v>78</v>
+      </c>
+      <c r="G117" t="n">
+        <v>77</v>
+      </c>
+      <c r="H117" t="n">
+        <v>70</v>
+      </c>
+      <c r="I117" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="1" t="n">
+        <v>116</v>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>Heather Hernandez</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>73366 Kelly Wells
+Jeremychester, MH 30560</t>
+        </is>
+      </c>
+      <c r="D118" t="n">
+        <v>67</v>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="F118" t="n">
+        <v>83</v>
+      </c>
+      <c r="G118" t="n">
+        <v>80</v>
+      </c>
+      <c r="H118" t="n">
+        <v>70</v>
+      </c>
+      <c r="I118" t="n">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="1" t="n">
+        <v>117</v>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>Jimmy Nelson</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>60888 Sanchez Hills
+Kevintown, IN 19701</t>
+        </is>
+      </c>
+      <c r="D119" t="n">
+        <v>53</v>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="F119" t="n">
+        <v>41</v>
+      </c>
+      <c r="G119" t="n">
+        <v>67</v>
+      </c>
+      <c r="H119" t="n">
+        <v>52</v>
+      </c>
+      <c r="I119" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="1" t="n">
+        <v>118</v>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>Julia Cameron</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>874 Lisa Brooks Apt. 369
+Lake Rachel, VI 71053</t>
+        </is>
+      </c>
+      <c r="D120" t="n">
+        <v>80</v>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="F120" t="n">
+        <v>76</v>
+      </c>
+      <c r="G120" t="n">
+        <v>58</v>
+      </c>
+      <c r="H120" t="n">
+        <v>99</v>
+      </c>
+      <c r="I120" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="1" t="n">
+        <v>119</v>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>Brittany Sullivan</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>Unit 1511 Box 7119
+DPO AA 13229</t>
+        </is>
+      </c>
+      <c r="D121" t="n">
+        <v>5</v>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="F121" t="n">
+        <v>96</v>
+      </c>
+      <c r="G121" t="n">
+        <v>61</v>
+      </c>
+      <c r="H121" t="n">
+        <v>67</v>
+      </c>
+      <c r="I121" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="1" t="n">
+        <v>120</v>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>Alice Wilson</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>1987 Christopher Orchard
+Lake Jamesside, VA 33763</t>
+        </is>
+      </c>
+      <c r="D122" t="n">
+        <v>15</v>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="F122" t="n">
+        <v>74</v>
+      </c>
+      <c r="G122" t="n">
+        <v>40</v>
+      </c>
+      <c r="H122" t="n">
+        <v>54</v>
+      </c>
+      <c r="I122" t="n">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="1" t="n">
+        <v>121</v>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>Thomas Reid</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>USCGC Reid
+FPO AP 38958</t>
+        </is>
+      </c>
+      <c r="D123" t="n">
+        <v>95</v>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="F123" t="n">
+        <v>61</v>
+      </c>
+      <c r="G123" t="n">
+        <v>47</v>
+      </c>
+      <c r="H123" t="n">
+        <v>92</v>
+      </c>
+      <c r="I123" t="n">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="1" t="n">
+        <v>122</v>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>Maurice Williams</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>1823 Jennifer Extension Apt. 167
+Lake Leebury, WV 28336</t>
+        </is>
+      </c>
+      <c r="D124" t="n">
+        <v>40</v>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="F124" t="n">
+        <v>63</v>
+      </c>
+      <c r="G124" t="n">
+        <v>68</v>
+      </c>
+      <c r="H124" t="n">
+        <v>79</v>
+      </c>
+      <c r="I124" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="1" t="n">
+        <v>123</v>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>Sandra Roberson</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>8607 Melissa Park Suite 053
+New Danielburgh, KY 14476</t>
+        </is>
+      </c>
+      <c r="D125" t="n">
+        <v>39</v>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="F125" t="n">
+        <v>87</v>
+      </c>
+      <c r="G125" t="n">
+        <v>67</v>
+      </c>
+      <c r="H125" t="n">
+        <v>67</v>
+      </c>
+      <c r="I125" t="n">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="1" t="n">
+        <v>124</v>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>Tracy Perez</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>78179 Simpson Valley Apt. 605
+Chambersmouth, OR 34646</t>
+        </is>
+      </c>
+      <c r="D126" t="n">
+        <v>47</v>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="F126" t="n">
+        <v>99</v>
+      </c>
+      <c r="G126" t="n">
+        <v>85</v>
+      </c>
+      <c r="H126" t="n">
+        <v>53</v>
+      </c>
+      <c r="I126" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="1" t="n">
+        <v>125</v>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>Kevin Anthony</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>18083 Stacy Run
+New Mary, GA 29053</t>
+        </is>
+      </c>
+      <c r="D127" t="n">
+        <v>82</v>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="F127" t="n">
+        <v>72</v>
+      </c>
+      <c r="G127" t="n">
+        <v>95</v>
+      </c>
+      <c r="H127" t="n">
+        <v>79</v>
+      </c>
+      <c r="I127" t="n">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="1" t="n">
+        <v>126</v>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>Ashley Bowers</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>863 Cook Parks
+Schneiderland, RI 50806</t>
+        </is>
+      </c>
+      <c r="D128" t="n">
+        <v>6</v>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="F128" t="n">
+        <v>65</v>
+      </c>
+      <c r="G128" t="n">
+        <v>70</v>
+      </c>
+      <c r="H128" t="n">
+        <v>85</v>
+      </c>
+      <c r="I128" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="1" t="n">
+        <v>127</v>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>Joshua Lopez</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>1287 Young Hill Suite 425
+Erikton, NY 61848</t>
+        </is>
+      </c>
+      <c r="D129" t="n">
+        <v>4</v>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="F129" t="n">
+        <v>62</v>
+      </c>
+      <c r="G129" t="n">
+        <v>42</v>
+      </c>
+      <c r="H129" t="n">
+        <v>77</v>
+      </c>
+      <c r="I129" t="n">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="1" t="n">
+        <v>128</v>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>Steven French</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>3232 Cox Points Apt. 912
+Miguelport, NH 67864</t>
+        </is>
+      </c>
+      <c r="D130" t="n">
+        <v>63</v>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="F130" t="n">
+        <v>59</v>
+      </c>
+      <c r="G130" t="n">
+        <v>90</v>
+      </c>
+      <c r="H130" t="n">
+        <v>44</v>
+      </c>
+      <c r="I130" t="n">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="1" t="n">
+        <v>129</v>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>James Murphy</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>USNV Obrien
+FPO AA 99513</t>
+        </is>
+      </c>
+      <c r="D131" t="n">
+        <v>87</v>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="F131" t="n">
+        <v>43</v>
+      </c>
+      <c r="G131" t="n">
+        <v>72</v>
+      </c>
+      <c r="H131" t="n">
+        <v>46</v>
+      </c>
+      <c r="I131" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="1" t="n">
+        <v>130</v>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>Anthony Aguilar</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>1974 Carolyn Trafficway Apt. 314
+South Lori, UT 24106</t>
+        </is>
+      </c>
+      <c r="D132" t="n">
+        <v>43</v>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="F132" t="n">
+        <v>93</v>
+      </c>
+      <c r="G132" t="n">
+        <v>47</v>
+      </c>
+      <c r="H132" t="n">
+        <v>94</v>
+      </c>
+      <c r="I132" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="1" t="n">
+        <v>131</v>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>Jocelyn Herman</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>3403 Debra Meadows
+New Cassandra, OK 86801</t>
+        </is>
+      </c>
+      <c r="D133" t="n">
+        <v>9</v>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="F133" t="n">
+        <v>86</v>
+      </c>
+      <c r="G133" t="n">
+        <v>70</v>
+      </c>
+      <c r="H133" t="n">
+        <v>88</v>
+      </c>
+      <c r="I133" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="1" t="n">
+        <v>132</v>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>Dana Murphy</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>0161 Sarah Prairie
+North Alyssa, UT 60842</t>
+        </is>
+      </c>
+      <c r="D134" t="n">
+        <v>7</v>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="F134" t="n">
+        <v>63</v>
+      </c>
+      <c r="G134" t="n">
+        <v>50</v>
+      </c>
+      <c r="H134" t="n">
+        <v>63</v>
+      </c>
+      <c r="I134" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="1" t="n">
+        <v>133</v>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>Stephen Andrews</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>136 Brenda Points
+Wilsonborough, IN 88663</t>
+        </is>
+      </c>
+      <c r="D135" t="n">
+        <v>29</v>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="F135" t="n">
+        <v>100</v>
+      </c>
+      <c r="G135" t="n">
+        <v>49</v>
+      </c>
+      <c r="H135" t="n">
+        <v>52</v>
+      </c>
+      <c r="I135" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="1" t="n">
+        <v>134</v>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>Craig Jones</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>39505 Allen Field Suite 562
+Vancemouth, ID 98166</t>
+        </is>
+      </c>
+      <c r="D136" t="n">
+        <v>68</v>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="F136" t="n">
+        <v>56</v>
+      </c>
+      <c r="G136" t="n">
+        <v>47</v>
+      </c>
+      <c r="H136" t="n">
+        <v>70</v>
+      </c>
+      <c r="I136" t="n">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="1" t="n">
+        <v>135</v>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>Denise Espinoza</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>6319 Hall Stravenue
+Alexisburgh, CO 62808</t>
+        </is>
+      </c>
+      <c r="D137" t="n">
+        <v>61</v>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="F137" t="n">
+        <v>78</v>
+      </c>
+      <c r="G137" t="n">
+        <v>50</v>
+      </c>
+      <c r="H137" t="n">
+        <v>41</v>
+      </c>
+      <c r="I137" t="n">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="1" t="n">
+        <v>136</v>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>Ms. Kim Torres</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>74155 Charles Stravenue Suite 932
+Stephanietown, WV 41777</t>
+        </is>
+      </c>
+      <c r="D138" t="n">
+        <v>89</v>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="F138" t="n">
+        <v>48</v>
+      </c>
+      <c r="G138" t="n">
+        <v>67</v>
+      </c>
+      <c r="H138" t="n">
+        <v>71</v>
+      </c>
+      <c r="I138" t="n">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="1" t="n">
+        <v>137</v>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>Crystal Cross</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>USNS Massey
+FPO AP 29126</t>
+        </is>
+      </c>
+      <c r="D139" t="n">
+        <v>11</v>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="F139" t="n">
+        <v>92</v>
+      </c>
+      <c r="G139" t="n">
+        <v>96</v>
+      </c>
+      <c r="H139" t="n">
+        <v>93</v>
+      </c>
+      <c r="I139" t="n">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="1" t="n">
+        <v>138</v>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>Leslie Schwartz</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>15691 Robert Plains Suite 293
+Chadport, DC 57024</t>
+        </is>
+      </c>
+      <c r="D140" t="n">
+        <v>37</v>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="F140" t="n">
+        <v>90</v>
+      </c>
+      <c r="G140" t="n">
+        <v>79</v>
+      </c>
+      <c r="H140" t="n">
+        <v>72</v>
+      </c>
+      <c r="I140" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="1" t="n">
+        <v>139</v>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>John Kennedy</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>1232 Ramirez Parkways
+Port Aprilmouth, OR 59520</t>
+        </is>
+      </c>
+      <c r="D141" t="n">
+        <v>55</v>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="F141" t="n">
+        <v>45</v>
+      </c>
+      <c r="G141" t="n">
+        <v>50</v>
+      </c>
+      <c r="H141" t="n">
+        <v>42</v>
+      </c>
+      <c r="I141" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>Samantha Cox</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>20534 Davis Knoll
+Lake Andres, CT 49596</t>
+        </is>
+      </c>
+      <c r="D142" t="n">
+        <v>33</v>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="F142" t="n">
+        <v>93</v>
+      </c>
+      <c r="G142" t="n">
+        <v>65</v>
+      </c>
+      <c r="H142" t="n">
+        <v>100</v>
+      </c>
+      <c r="I142" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="1" t="n">
+        <v>141</v>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>Bridget Bradley</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>Unit 2189 Box 4218
+DPO AP 61875</t>
+        </is>
+      </c>
+      <c r="D143" t="n">
+        <v>60</v>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="F143" t="n">
+        <v>71</v>
+      </c>
+      <c r="G143" t="n">
+        <v>47</v>
+      </c>
+      <c r="H143" t="n">
+        <v>78</v>
+      </c>
+      <c r="I143" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="1" t="n">
+        <v>142</v>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>Joshua Jones</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>9365 Claire Lodge
+Alyssastad, OR 03462</t>
+        </is>
+      </c>
+      <c r="D144" t="n">
+        <v>72</v>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="F144" t="n">
+        <v>78</v>
+      </c>
+      <c r="G144" t="n">
+        <v>41</v>
+      </c>
+      <c r="H144" t="n">
+        <v>69</v>
+      </c>
+      <c r="I144" t="n">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="1" t="n">
+        <v>143</v>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>Stacey Jimenez</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>0244 Peterson Prairie Apt. 792
+Stevensmouth, IA 73532</t>
+        </is>
+      </c>
+      <c r="D145" t="n">
+        <v>86</v>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="F145" t="n">
+        <v>96</v>
+      </c>
+      <c r="G145" t="n">
+        <v>80</v>
+      </c>
+      <c r="H145" t="n">
+        <v>42</v>
+      </c>
+      <c r="I145" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="1" t="n">
+        <v>144</v>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>Alexandra Benton</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>6450 Blake Mount
+Ericland, KY 33926</t>
+        </is>
+      </c>
+      <c r="D146" t="n">
+        <v>74</v>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="F146" t="n">
+        <v>84</v>
+      </c>
+      <c r="G146" t="n">
+        <v>85</v>
+      </c>
+      <c r="H146" t="n">
+        <v>53</v>
+      </c>
+      <c r="I146" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>Eric Garcia</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>67589 Scott River
+Butlerville, AK 68969</t>
+        </is>
+      </c>
+      <c r="D147" t="n">
+        <v>45</v>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="F147" t="n">
+        <v>87</v>
+      </c>
+      <c r="G147" t="n">
+        <v>76</v>
+      </c>
+      <c r="H147" t="n">
+        <v>40</v>
+      </c>
+      <c r="I147" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="1" t="n">
+        <v>146</v>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>Sarah Brown</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>565 Jeremiah Fields
+South Jeanette, AK 97650</t>
+        </is>
+      </c>
+      <c r="D148" t="n">
+        <v>19</v>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="F148" t="n">
+        <v>57</v>
+      </c>
+      <c r="G148" t="n">
+        <v>97</v>
+      </c>
+      <c r="H148" t="n">
+        <v>41</v>
+      </c>
+      <c r="I148" t="n">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="1" t="n">
+        <v>147</v>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>Brianna Rios MD</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>PSC 9036, Box 0781
+APO AE 73816</t>
+        </is>
+      </c>
+      <c r="D149" t="n">
+        <v>16</v>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="F149" t="n">
+        <v>69</v>
+      </c>
+      <c r="G149" t="n">
+        <v>41</v>
+      </c>
+      <c r="H149" t="n">
+        <v>64</v>
+      </c>
+      <c r="I149" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="1" t="n">
+        <v>148</v>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>Patricia Schneider</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>862 Middleton Union
+Woodburgh, AR 17504</t>
+        </is>
+      </c>
+      <c r="D150" t="n">
+        <v>56</v>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="F150" t="n">
+        <v>93</v>
+      </c>
+      <c r="G150" t="n">
+        <v>87</v>
+      </c>
+      <c r="H150" t="n">
+        <v>90</v>
+      </c>
+      <c r="I150" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="1" t="n">
+        <v>149</v>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>Justin Ware</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>341 Joy Lakes Suite 776
+Lake Alexisville, VA 09309</t>
+        </is>
+      </c>
+      <c r="D151" t="n">
+        <v>83</v>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="F151" t="n">
+        <v>97</v>
+      </c>
+      <c r="G151" t="n">
+        <v>56</v>
+      </c>
+      <c r="H151" t="n">
+        <v>71</v>
+      </c>
+      <c r="I151" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>Albert Allen DDS</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>25401 Belinda Forges
+West Carlosberg, MS 28243</t>
+        </is>
+      </c>
+      <c r="D152" t="n">
+        <v>90</v>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="F152" t="n">
+        <v>65</v>
+      </c>
+      <c r="G152" t="n">
+        <v>60</v>
+      </c>
+      <c r="H152" t="n">
+        <v>80</v>
+      </c>
+      <c r="I152" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="1" t="n">
+        <v>151</v>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>Heather Cunningham</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>026 Micheal Point
+Farmerland, CO 28740</t>
+        </is>
+      </c>
+      <c r="D153" t="n">
+        <v>13</v>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="F153" t="n">
+        <v>46</v>
+      </c>
+      <c r="G153" t="n">
+        <v>70</v>
+      </c>
+      <c r="H153" t="n">
+        <v>52</v>
+      </c>
+      <c r="I153" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="1" t="n">
+        <v>152</v>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>Katrina Rodriguez</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>42764 Ross Roads
+Wolfville, ID 84485</t>
+        </is>
+      </c>
+      <c r="D154" t="n">
+        <v>79</v>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="F154" t="n">
+        <v>40</v>
+      </c>
+      <c r="G154" t="n">
+        <v>49</v>
+      </c>
+      <c r="H154" t="n">
+        <v>49</v>
+      </c>
+      <c r="I154" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="1" t="n">
+        <v>153</v>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>Taylor Horton</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>2482 Jane Spur
+Robertberg, MO 72099</t>
+        </is>
+      </c>
+      <c r="D155" t="n">
+        <v>35</v>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="F155" t="n">
+        <v>55</v>
+      </c>
+      <c r="G155" t="n">
+        <v>43</v>
+      </c>
+      <c r="H155" t="n">
+        <v>48</v>
+      </c>
+      <c r="I155" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="1" t="n">
+        <v>154</v>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>Ryan Chavez</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>75681 Baird Shoal Apt. 745
+Smithfurt, MN 99210</t>
+        </is>
+      </c>
+      <c r="D156" t="n">
+        <v>78</v>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="F156" t="n">
+        <v>63</v>
+      </c>
+      <c r="G156" t="n">
+        <v>94</v>
+      </c>
+      <c r="H156" t="n">
+        <v>87</v>
+      </c>
+      <c r="I156" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" s="1" t="n">
+        <v>155</v>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>Sheila Martinez</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>428 Reese Knolls
+Port Kevin, ND 38559</t>
+        </is>
+      </c>
+      <c r="D157" t="n">
+        <v>92</v>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="F157" t="n">
+        <v>55</v>
+      </c>
+      <c r="G157" t="n">
+        <v>93</v>
+      </c>
+      <c r="H157" t="n">
+        <v>87</v>
+      </c>
+      <c r="I157" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="1" t="n">
+        <v>156</v>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>Tiffany Colon</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>94535 Harris Rapid
+East Calvin, ID 10729</t>
+        </is>
+      </c>
+      <c r="D158" t="n">
+        <v>85</v>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="F158" t="n">
+        <v>61</v>
+      </c>
+      <c r="G158" t="n">
+        <v>95</v>
+      </c>
+      <c r="H158" t="n">
+        <v>60</v>
+      </c>
+      <c r="I158" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" s="1" t="n">
+        <v>157</v>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>Rachel Rush</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>2493 James Fort
+Richardsonview, AL 65990</t>
+        </is>
+      </c>
+      <c r="D159" t="n">
+        <v>26</v>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="F159" t="n">
+        <v>78</v>
+      </c>
+      <c r="G159" t="n">
+        <v>66</v>
+      </c>
+      <c r="H159" t="n">
+        <v>71</v>
+      </c>
+      <c r="I159" t="n">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="1" t="n">
+        <v>158</v>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>Patrick Clements</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>280 Ian Mountain
+Brandonstad, MN 90864</t>
+        </is>
+      </c>
+      <c r="D160" t="n">
+        <v>21</v>
+      </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="F160" t="n">
+        <v>68</v>
+      </c>
+      <c r="G160" t="n">
+        <v>100</v>
+      </c>
+      <c r="H160" t="n">
+        <v>71</v>
+      </c>
+      <c r="I160" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="1" t="n">
+        <v>159</v>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>Robert Castillo</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>9102 Keith Causeway Suite 074
+East Aprilport, ND 30507</t>
+        </is>
+      </c>
+      <c r="D161" t="n">
+        <v>75</v>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="F161" t="n">
+        <v>65</v>
+      </c>
+      <c r="G161" t="n">
+        <v>56</v>
+      </c>
+      <c r="H161" t="n">
+        <v>96</v>
+      </c>
+      <c r="I161" t="n">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="1" t="n">
+        <v>160</v>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>Jonathan Larsen</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>257 Thomas Ports
+North Ashleystad, IA 62111</t>
+        </is>
+      </c>
+      <c r="D162" t="n">
+        <v>77</v>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="F162" t="n">
+        <v>80</v>
+      </c>
+      <c r="G162" t="n">
+        <v>58</v>
+      </c>
+      <c r="H162" t="n">
+        <v>92</v>
+      </c>
+      <c r="I162" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="1" t="n">
+        <v>161</v>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>Lacey Cherry</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>36716 Taylor Trafficway Apt. 318
+Mckinneymouth, UT 48070</t>
+        </is>
+      </c>
+      <c r="D163" t="n">
+        <v>3</v>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="F163" t="n">
+        <v>50</v>
+      </c>
+      <c r="G163" t="n">
+        <v>53</v>
+      </c>
+      <c r="H163" t="n">
+        <v>60</v>
+      </c>
+      <c r="I163" t="n">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="1" t="n">
+        <v>162</v>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>Jessica Lewis</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>3662 Key Streets Apt. 071
+Carrbury, GA 39242</t>
+        </is>
+      </c>
+      <c r="D164" t="n">
+        <v>96</v>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="F164" t="n">
+        <v>90</v>
+      </c>
+      <c r="G164" t="n">
+        <v>64</v>
+      </c>
+      <c r="H164" t="n">
+        <v>54</v>
+      </c>
+      <c r="I164" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" s="1" t="n">
+        <v>163</v>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>Matthew King</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>0665 Pamela Stravenue Suite 525
+Millerland, HI 56640</t>
+        </is>
+      </c>
+      <c r="D165" t="n">
+        <v>42</v>
+      </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="F165" t="n">
+        <v>74</v>
+      </c>
+      <c r="G165" t="n">
+        <v>85</v>
+      </c>
+      <c r="H165" t="n">
+        <v>62</v>
+      </c>
+      <c r="I165" t="n">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="1" t="n">
+        <v>164</v>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>Stephanie Fuller</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>33685 Selena Points Apt. 577
+Munozville, IN 53438</t>
+        </is>
+      </c>
+      <c r="D166" t="n">
+        <v>46</v>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="F166" t="n">
+        <v>60</v>
+      </c>
+      <c r="G166" t="n">
+        <v>78</v>
+      </c>
+      <c r="H166" t="n">
+        <v>88</v>
+      </c>
+      <c r="I166" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="1" t="n">
+        <v>165</v>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>Shawn Bullock</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>443 Clark Alley
+North Frederickport, OH 17072</t>
+        </is>
+      </c>
+      <c r="D167" t="n">
+        <v>98</v>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="F167" t="n">
+        <v>100</v>
+      </c>
+      <c r="G167" t="n">
+        <v>72</v>
+      </c>
+      <c r="H167" t="n">
+        <v>64</v>
+      </c>
+      <c r="I167" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="1" t="n">
+        <v>166</v>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>Jordan Price</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>287 Strickland Lane
+Jamieshire, OH 71665</t>
+        </is>
+      </c>
+      <c r="D168" t="n">
+        <v>62</v>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="F168" t="n">
+        <v>75</v>
+      </c>
+      <c r="G168" t="n">
+        <v>67</v>
+      </c>
+      <c r="H168" t="n">
+        <v>53</v>
+      </c>
+      <c r="I168" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" s="1" t="n">
+        <v>167</v>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>Stephanie Garcia</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>10710 Wagner Pass
+East Meghanstad, SC 53056</t>
+        </is>
+      </c>
+      <c r="D169" t="n">
+        <v>100</v>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="F169" t="n">
+        <v>40</v>
+      </c>
+      <c r="G169" t="n">
+        <v>47</v>
+      </c>
+      <c r="H169" t="n">
+        <v>59</v>
+      </c>
+      <c r="I169" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" s="1" t="n">
+        <v>168</v>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>Mrs. Angela Sullivan</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>231 Karen Shores
+Port Davidmouth, GU 63124</t>
+        </is>
+      </c>
+      <c r="D170" t="n">
+        <v>99</v>
+      </c>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="F170" t="n">
+        <v>76</v>
+      </c>
+      <c r="G170" t="n">
+        <v>44</v>
+      </c>
+      <c r="H170" t="n">
+        <v>98</v>
+      </c>
+      <c r="I170" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" s="1" t="n">
+        <v>169</v>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>Andrew Werner</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>832 Quinn Estates
+Robertberg, NY 40633</t>
+        </is>
+      </c>
+      <c r="D171" t="n">
+        <v>12</v>
+      </c>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="F171" t="n">
+        <v>79</v>
+      </c>
+      <c r="G171" t="n">
+        <v>45</v>
+      </c>
+      <c r="H171" t="n">
+        <v>85</v>
+      </c>
+      <c r="I171" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" s="1" t="n">
+        <v>170</v>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>Christopher Davis</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>50536 Ebony Run
+Jasonborough, DC 41145</t>
+        </is>
+      </c>
+      <c r="D172" t="n">
+        <v>32</v>
+      </c>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="F172" t="n">
+        <v>70</v>
+      </c>
+      <c r="G172" t="n">
+        <v>89</v>
+      </c>
+      <c r="H172" t="n">
+        <v>69</v>
+      </c>
+      <c r="I172" t="n">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" s="1" t="n">
+        <v>171</v>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>Geoffrey Ingram</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>9953 Shaffer Junctions Suite 700
+East Davidport, AK 24541</t>
+        </is>
+      </c>
+      <c r="D173" t="n">
+        <v>65</v>
+      </c>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="F173" t="n">
+        <v>82</v>
+      </c>
+      <c r="G173" t="n">
+        <v>41</v>
+      </c>
+      <c r="H173" t="n">
+        <v>81</v>
+      </c>
+      <c r="I173" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" s="1" t="n">
+        <v>172</v>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>Bryan Jones</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>7613 Mark Point Apt. 710
+Brandimouth, ME 05240</t>
+        </is>
+      </c>
+      <c r="D174" t="n">
+        <v>50</v>
+      </c>
+      <c r="E174" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="F174" t="n">
+        <v>52</v>
+      </c>
+      <c r="G174" t="n">
+        <v>71</v>
+      </c>
+      <c r="H174" t="n">
+        <v>44</v>
+      </c>
+      <c r="I174" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="1" t="n">
+        <v>173</v>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>Heather Martinez</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>USNS Good
+FPO AP 61919</t>
+        </is>
+      </c>
+      <c r="D175" t="n">
+        <v>91</v>
+      </c>
+      <c r="E175" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="F175" t="n">
+        <v>90</v>
+      </c>
+      <c r="G175" t="n">
+        <v>84</v>
+      </c>
+      <c r="H175" t="n">
+        <v>98</v>
+      </c>
+      <c r="I175" t="n">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="1" t="n">
+        <v>174</v>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>Christopher Clayton</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>PSC 2521, Box 8070
+APO AE 72112</t>
+        </is>
+      </c>
+      <c r="D176" t="n">
+        <v>18</v>
+      </c>
+      <c r="E176" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="F176" t="n">
+        <v>62</v>
+      </c>
+      <c r="G176" t="n">
+        <v>40</v>
+      </c>
+      <c r="H176" t="n">
+        <v>55</v>
+      </c>
+      <c r="I176" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" s="1" t="n">
+        <v>175</v>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>Debbie Herrera</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>PSC 1502, Box 3042
+APO AA 24219</t>
+        </is>
+      </c>
+      <c r="D177" t="n">
+        <v>10</v>
+      </c>
+      <c r="E177" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="F177" t="n">
+        <v>91</v>
+      </c>
+      <c r="G177" t="n">
+        <v>72</v>
+      </c>
+      <c r="H177" t="n">
+        <v>55</v>
+      </c>
+      <c r="I177" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="1" t="n">
+        <v>176</v>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>William Woods</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>Unit 9615 Box 5176
+DPO AE 41863</t>
+        </is>
+      </c>
+      <c r="D178" t="n">
+        <v>59</v>
+      </c>
+      <c r="E178" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="F178" t="n">
+        <v>57</v>
+      </c>
+      <c r="G178" t="n">
+        <v>97</v>
+      </c>
+      <c r="H178" t="n">
+        <v>95</v>
+      </c>
+      <c r="I178" t="n">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="1" t="n">
+        <v>177</v>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>Courtney Thompson</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>091 Aaron Trace
+Castilloside, KS 04880</t>
+        </is>
+      </c>
+      <c r="D179" t="n">
+        <v>41</v>
+      </c>
+      <c r="E179" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="F179" t="n">
+        <v>82</v>
+      </c>
+      <c r="G179" t="n">
+        <v>61</v>
+      </c>
+      <c r="H179" t="n">
+        <v>93</v>
+      </c>
+      <c r="I179" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="1" t="n">
+        <v>178</v>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>Charles Jordan</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>776 Chad Manors Suite 516
+Davismouth, DE 08053</t>
+        </is>
+      </c>
+      <c r="D180" t="n">
+        <v>69</v>
+      </c>
+      <c r="E180" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="F180" t="n">
+        <v>68</v>
+      </c>
+      <c r="G180" t="n">
+        <v>72</v>
+      </c>
+      <c r="H180" t="n">
+        <v>52</v>
+      </c>
+      <c r="I180" t="n">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" s="1" t="n">
+        <v>179</v>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>Andrew Gallagher</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>941 Jennifer Key Suite 932
+Lake Andrew, DC 33474</t>
+        </is>
+      </c>
+      <c r="D181" t="n">
+        <v>36</v>
+      </c>
+      <c r="E181" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="F181" t="n">
+        <v>92</v>
+      </c>
+      <c r="G181" t="n">
+        <v>69</v>
+      </c>
+      <c r="H181" t="n">
+        <v>49</v>
+      </c>
+      <c r="I181" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" s="1" t="n">
+        <v>180</v>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>James Compton</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>222 Ramirez Avenue Suite 033
+Nelsonshire, RI 23352</t>
+        </is>
+      </c>
+      <c r="D182" t="n">
+        <v>84</v>
+      </c>
+      <c r="E182" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="F182" t="n">
+        <v>89</v>
+      </c>
+      <c r="G182" t="n">
+        <v>60</v>
+      </c>
+      <c r="H182" t="n">
+        <v>48</v>
+      </c>
+      <c r="I182" t="n">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" s="1" t="n">
+        <v>181</v>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>Bethany Grimes</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>PSC 4072, Box 1133
+APO AA 58033</t>
+        </is>
+      </c>
+      <c r="D183" t="n">
+        <v>76</v>
+      </c>
+      <c r="E183" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="F183" t="n">
+        <v>77</v>
+      </c>
+      <c r="G183" t="n">
+        <v>74</v>
+      </c>
+      <c r="H183" t="n">
+        <v>82</v>
+      </c>
+      <c r="I183" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" s="1" t="n">
+        <v>182</v>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>Lisa Morgan</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>81347 Joshua Stravenue Apt. 520
+Hernandeztown, IL 36403</t>
+        </is>
+      </c>
+      <c r="D184" t="n">
+        <v>48</v>
+      </c>
+      <c r="E184" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="F184" t="n">
+        <v>51</v>
+      </c>
+      <c r="G184" t="n">
+        <v>65</v>
+      </c>
+      <c r="H184" t="n">
+        <v>46</v>
+      </c>
+      <c r="I184" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" s="1" t="n">
+        <v>183</v>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>Cesar Simmons</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>286 Deborah Valley
+West Sean, NJ 51138</t>
+        </is>
+      </c>
+      <c r="D185" t="n">
+        <v>17</v>
+      </c>
+      <c r="E185" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="F185" t="n">
+        <v>66</v>
+      </c>
+      <c r="G185" t="n">
+        <v>44</v>
+      </c>
+      <c r="H185" t="n">
+        <v>55</v>
+      </c>
+      <c r="I185" t="n">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" s="1" t="n">
+        <v>184</v>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>Amanda Jackson</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>2086 Patricia Mountain
+Lake Stephenstad, NV 88809</t>
+        </is>
+      </c>
+      <c r="D186" t="n">
+        <v>64</v>
+      </c>
+      <c r="E186" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="F186" t="n">
+        <v>58</v>
+      </c>
+      <c r="G186" t="n">
+        <v>53</v>
+      </c>
+      <c r="H186" t="n">
+        <v>80</v>
+      </c>
+      <c r="I186" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" s="1" t="n">
+        <v>185</v>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>Michael Bennett</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>3970 Anthony Glen
+Ramirezchester, SC 08256</t>
+        </is>
+      </c>
+      <c r="D187" t="n">
+        <v>88</v>
+      </c>
+      <c r="E187" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="F187" t="n">
+        <v>92</v>
+      </c>
+      <c r="G187" t="n">
+        <v>82</v>
+      </c>
+      <c r="H187" t="n">
+        <v>60</v>
+      </c>
+      <c r="I187" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" s="1" t="n">
+        <v>186</v>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>Chelsey Perkins</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>USNV Mcclain
+FPO AP 65975</t>
+        </is>
+      </c>
+      <c r="D188" t="n">
+        <v>38</v>
+      </c>
+      <c r="E188" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="F188" t="n">
+        <v>89</v>
+      </c>
+      <c r="G188" t="n">
+        <v>89</v>
+      </c>
+      <c r="H188" t="n">
+        <v>86</v>
+      </c>
+      <c r="I188" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" s="1" t="n">
+        <v>187</v>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>Christopher Collins</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>4348 Frey Walk
+Tracyfurt, SC 68872</t>
+        </is>
+      </c>
+      <c r="D189" t="n">
+        <v>27</v>
+      </c>
+      <c r="E189" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="F189" t="n">
+        <v>40</v>
+      </c>
+      <c r="G189" t="n">
+        <v>45</v>
+      </c>
+      <c r="H189" t="n">
+        <v>46</v>
+      </c>
+      <c r="I189" t="n">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" s="1" t="n">
+        <v>188</v>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>Morgan Buchanan</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>725 Miller Shoal Apt. 115
+West Hannah, HI 53216</t>
+        </is>
+      </c>
+      <c r="D190" t="n">
+        <v>25</v>
+      </c>
+      <c r="E190" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="F190" t="n">
+        <v>59</v>
+      </c>
+      <c r="G190" t="n">
+        <v>95</v>
+      </c>
+      <c r="H190" t="n">
+        <v>75</v>
+      </c>
+      <c r="I190" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" s="1" t="n">
+        <v>189</v>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>Patrick Phillips</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>PSC 2362, Box 8632
+APO AE 01068</t>
+        </is>
+      </c>
+      <c r="D191" t="n">
+        <v>52</v>
+      </c>
+      <c r="E191" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="F191" t="n">
+        <v>49</v>
+      </c>
+      <c r="G191" t="n">
+        <v>79</v>
+      </c>
+      <c r="H191" t="n">
+        <v>76</v>
+      </c>
+      <c r="I191" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" s="1" t="n">
+        <v>190</v>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>Elizabeth Robinson</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>9159 Hill Stream Apt. 761
+South Johnathan, MS 10488</t>
+        </is>
+      </c>
+      <c r="D192" t="n">
+        <v>30</v>
+      </c>
+      <c r="E192" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="F192" t="n">
+        <v>78</v>
+      </c>
+      <c r="G192" t="n">
+        <v>78</v>
+      </c>
+      <c r="H192" t="n">
+        <v>89</v>
+      </c>
+      <c r="I192" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" s="1" t="n">
+        <v>191</v>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>Richard Russell</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>5943 Kristen Village
+Danielton, UT 49680</t>
+        </is>
+      </c>
+      <c r="D193" t="n">
+        <v>54</v>
+      </c>
+      <c r="E193" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="F193" t="n">
+        <v>76</v>
+      </c>
+      <c r="G193" t="n">
+        <v>77</v>
+      </c>
+      <c r="H193" t="n">
+        <v>97</v>
+      </c>
+      <c r="I193" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" s="1" t="n">
+        <v>192</v>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>Benjamin Woods</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>8531 Estrada Trafficway Suite 748
+North Traceymouth, PA 87909</t>
+        </is>
+      </c>
+      <c r="D194" t="n">
+        <v>31</v>
+      </c>
+      <c r="E194" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="F194" t="n">
+        <v>42</v>
+      </c>
+      <c r="G194" t="n">
+        <v>68</v>
+      </c>
+      <c r="H194" t="n">
+        <v>88</v>
+      </c>
+      <c r="I194" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" s="1" t="n">
+        <v>193</v>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>Mary Rivas</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>05764 Moore Rest
+Costaport, MN 16640</t>
+        </is>
+      </c>
+      <c r="D195" t="n">
+        <v>22</v>
+      </c>
+      <c r="E195" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="F195" t="n">
+        <v>49</v>
+      </c>
+      <c r="G195" t="n">
+        <v>62</v>
+      </c>
+      <c r="H195" t="n">
+        <v>65</v>
+      </c>
+      <c r="I195" t="n">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" s="1" t="n">
+        <v>194</v>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>Adam Jackson</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>4538 Linda Glen Apt. 796
+Kathychester, MA 85070</t>
+        </is>
+      </c>
+      <c r="D196" t="n">
+        <v>49</v>
+      </c>
+      <c r="E196" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="F196" t="n">
+        <v>70</v>
+      </c>
+      <c r="G196" t="n">
+        <v>90</v>
+      </c>
+      <c r="H196" t="n">
+        <v>97</v>
+      </c>
+      <c r="I196" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" s="1" t="n">
+        <v>195</v>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>Larry Combs</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>161 Kimberly Row
+Leachhaven, DE 05382</t>
+        </is>
+      </c>
+      <c r="D197" t="n">
+        <v>66</v>
+      </c>
+      <c r="E197" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="F197" t="n">
+        <v>70</v>
+      </c>
+      <c r="G197" t="n">
+        <v>54</v>
+      </c>
+      <c r="H197" t="n">
+        <v>80</v>
+      </c>
+      <c r="I197" t="n">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" s="1" t="n">
+        <v>196</v>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>Laura Curtis</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>3784 Kevin Summit Suite 249
+North Jessica, NV 51792</t>
+        </is>
+      </c>
+      <c r="D198" t="n">
+        <v>8</v>
+      </c>
+      <c r="E198" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="F198" t="n">
+        <v>45</v>
+      </c>
+      <c r="G198" t="n">
+        <v>57</v>
+      </c>
+      <c r="H198" t="n">
+        <v>87</v>
+      </c>
+      <c r="I198" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" s="1" t="n">
+        <v>197</v>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>Hayley Hickman</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>74105 Thomas Square Apt. 634
+Hendricksstad, NE 40208</t>
+        </is>
+      </c>
+      <c r="D199" t="n">
+        <v>23</v>
+      </c>
+      <c r="E199" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="F199" t="n">
+        <v>67</v>
+      </c>
+      <c r="G199" t="n">
+        <v>59</v>
+      </c>
+      <c r="H199" t="n">
+        <v>85</v>
+      </c>
+      <c r="I199" t="n">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" s="1" t="n">
+        <v>198</v>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>Patricia Graves</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>3243 James Throughway
+Mcdanielberg, MN 06674</t>
+        </is>
+      </c>
+      <c r="D200" t="n">
+        <v>81</v>
+      </c>
+      <c r="E200" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="F200" t="n">
+        <v>89</v>
+      </c>
+      <c r="G200" t="n">
+        <v>81</v>
+      </c>
+      <c r="H200" t="n">
+        <v>84</v>
+      </c>
+      <c r="I200" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" s="1" t="n">
+        <v>199</v>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>Ryan Allen</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>4573 Clarke Divide Suite 644
+Port Stephanie, IL 30295</t>
+        </is>
+      </c>
+      <c r="D201" t="n">
+        <v>14</v>
+      </c>
+      <c r="E201" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="F201" t="n">
+        <v>71</v>
+      </c>
+      <c r="G201" t="n">
+        <v>52</v>
+      </c>
+      <c r="H201" t="n">
+        <v>99</v>
+      </c>
+      <c r="I201" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>Ryan Kelly</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>2108 Tran Mission Apt. 895
+West Meganstad, AL 20588</t>
+        </is>
+      </c>
+      <c r="D202" t="n">
+        <v>57</v>
+      </c>
+      <c r="E202" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="F202" t="n">
+        <v>100</v>
+      </c>
+      <c r="G202" t="n">
+        <v>64</v>
+      </c>
+      <c r="H202" t="n">
+        <v>63</v>
+      </c>
+      <c r="I202" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" s="1" t="n">
+        <v>201</v>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>Andrea Ramirez</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>066 Hayes Forges
+Sharonton, HI 52724</t>
+        </is>
+      </c>
+      <c r="D203" t="n">
+        <v>20</v>
+      </c>
+      <c r="E203" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="F203" t="n">
+        <v>63</v>
+      </c>
+      <c r="G203" t="n">
+        <v>89</v>
+      </c>
+      <c r="H203" t="n">
+        <v>61</v>
+      </c>
+      <c r="I203" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" s="1" t="n">
+        <v>202</v>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>James Howard</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>8859 Michelle Stream Apt. 773
+Whitebury, MP 55913</t>
+        </is>
+      </c>
+      <c r="D204" t="n">
+        <v>2</v>
+      </c>
+      <c r="E204" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="F204" t="n">
+        <v>85</v>
+      </c>
+      <c r="G204" t="n">
+        <v>60</v>
+      </c>
+      <c r="H204" t="n">
+        <v>46</v>
+      </c>
+      <c r="I204" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" s="1" t="n">
+        <v>203</v>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>Andrea Warner</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>Unit 4344 Box 1189
+DPO AP 65499</t>
+        </is>
+      </c>
+      <c r="D205" t="n">
+        <v>44</v>
+      </c>
+      <c r="E205" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="F205" t="n">
+        <v>90</v>
+      </c>
+      <c r="G205" t="n">
+        <v>73</v>
+      </c>
+      <c r="H205" t="n">
+        <v>61</v>
+      </c>
+      <c r="I205" t="n">
         <v>40</v>
       </c>
     </row>

</xml_diff>